<commit_message>
add description of new function
</commit_message>
<xml_diff>
--- a/description.xlsx
+++ b/description.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="221">
   <si>
     <t>SET_ORI(W,P,R)</t>
   </si>
@@ -679,6 +679,20 @@
 A матрица постоянных коэф. 
 D матрица где в первом столбце указаны правый части уравнений системы
 результат матрица где в первом стобце находятся решения матрицы</t>
+  </si>
+  <si>
+    <t>MATH_LIB. Cross_PNT (Line_frame, Plate_frame: XYZWPR): XYZWPR</t>
+  </si>
+  <si>
+    <t>вычисляет точку пересения Z оcи LINE_frame c XY плоскостью Plate_frame</t>
+  </si>
+  <si>
+    <t>MATH_LIB. Cross_Line (Plate1, Plate2: XYZWPR): XYZWPR</t>
+  </si>
+  <si>
+    <t>вычисляет фрейм X ось которого совпадает с прямой  пересения XY плоскости Plate1 и  XY плоскости Plate2. 
+Плоскость XY нового фрейма совпадает с плоскостью XY Plate1. 
+Начало отсчета новой системы находится на проекции начала Plate1 на прямую пересечения плоскостей</t>
   </si>
 </sst>
 </file>
@@ -1896,11 +1910,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C182" sqref="C182"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3893,72 +3907,72 @@
       <c r="E160" s="17"/>
       <c r="F160" s="86"/>
     </row>
-    <row r="161" spans="1:6" ht="15" customHeight="1">
-      <c r="A161" s="151" t="s">
+    <row r="161" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A161" s="104" t="s">
+        <v>217</v>
+      </c>
+      <c r="B161" s="15"/>
+      <c r="C161" s="14"/>
+      <c r="D161" s="14"/>
+      <c r="E161" s="14"/>
+      <c r="F161" s="84" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A162" s="105"/>
+      <c r="B162" s="21"/>
+      <c r="C162" s="31"/>
+      <c r="D162" s="31"/>
+      <c r="E162" s="31"/>
+      <c r="F162" s="85"/>
+    </row>
+    <row r="163" spans="1:6" ht="20.25" customHeight="1" thickBot="1">
+      <c r="A163" s="106"/>
+      <c r="B163" s="16"/>
+      <c r="C163" s="17"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="86"/>
+    </row>
+    <row r="164" spans="1:6" ht="60" customHeight="1">
+      <c r="A164" s="104" t="s">
+        <v>219</v>
+      </c>
+      <c r="B164" s="15"/>
+      <c r="C164" s="14"/>
+      <c r="D164" s="14"/>
+      <c r="E164" s="14"/>
+      <c r="F164" s="161" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="60" customHeight="1">
+      <c r="A165" s="105"/>
+      <c r="B165" s="21"/>
+      <c r="C165" s="31"/>
+      <c r="D165" s="31"/>
+      <c r="E165" s="31"/>
+      <c r="F165" s="162"/>
+    </row>
+    <row r="166" spans="1:6" ht="60" customHeight="1" thickBot="1">
+      <c r="A166" s="106"/>
+      <c r="B166" s="16"/>
+      <c r="C166" s="17"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="163"/>
+    </row>
+    <row r="167" spans="1:6" ht="15" customHeight="1">
+      <c r="A167" s="151" t="s">
         <v>203</v>
       </c>
-      <c r="B161" s="155"/>
-      <c r="C161" s="152"/>
-      <c r="D161" s="158"/>
-      <c r="E161" s="152"/>
-      <c r="F161" s="84" t="s">
+      <c r="B167" s="155"/>
+      <c r="C167" s="152"/>
+      <c r="D167" s="158"/>
+      <c r="E167" s="152"/>
+      <c r="F167" s="84" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
-      <c r="A162" s="149"/>
-      <c r="B162" s="156"/>
-      <c r="C162" s="153"/>
-      <c r="D162" s="159"/>
-      <c r="E162" s="153"/>
-      <c r="F162" s="85"/>
-    </row>
-    <row r="163" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A163" s="150"/>
-      <c r="B163" s="157"/>
-      <c r="C163" s="154"/>
-      <c r="D163" s="160"/>
-      <c r="E163" s="154"/>
-      <c r="F163" s="86"/>
-    </row>
-    <row r="164" spans="1:6">
-      <c r="A164" s="151" t="s">
-        <v>204</v>
-      </c>
-      <c r="B164" s="155"/>
-      <c r="C164" s="152"/>
-      <c r="D164" s="158"/>
-      <c r="E164" s="152"/>
-      <c r="F164" s="84" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6">
-      <c r="A165" s="149"/>
-      <c r="B165" s="156"/>
-      <c r="C165" s="153"/>
-      <c r="D165" s="159"/>
-      <c r="E165" s="153"/>
-      <c r="F165" s="85"/>
-    </row>
-    <row r="166" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A166" s="150"/>
-      <c r="B166" s="157"/>
-      <c r="C166" s="154"/>
-      <c r="D166" s="160"/>
-      <c r="E166" s="154"/>
-      <c r="F166" s="86"/>
-    </row>
-    <row r="167" spans="1:6">
-      <c r="A167" s="149" t="s">
-        <v>205</v>
-      </c>
-      <c r="B167" s="156"/>
-      <c r="C167" s="153"/>
-      <c r="D167" s="159"/>
-      <c r="E167" s="153"/>
-      <c r="F167" s="84" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -3970,23 +3984,23 @@
       <c r="F168" s="85"/>
     </row>
     <row r="169" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A169" s="149"/>
-      <c r="B169" s="156"/>
-      <c r="C169" s="153"/>
-      <c r="D169" s="159"/>
-      <c r="E169" s="153"/>
+      <c r="A169" s="150"/>
+      <c r="B169" s="157"/>
+      <c r="C169" s="154"/>
+      <c r="D169" s="160"/>
+      <c r="E169" s="154"/>
       <c r="F169" s="86"/>
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="151" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B170" s="155"/>
       <c r="C170" s="152"/>
       <c r="D170" s="158"/>
       <c r="E170" s="152"/>
       <c r="F170" s="84" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -4007,14 +4021,14 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="149" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B173" s="156"/>
       <c r="C173" s="153"/>
       <c r="D173" s="159"/>
       <c r="E173" s="153"/>
       <c r="F173" s="84" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -4035,14 +4049,14 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" s="151" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B176" s="155"/>
       <c r="C176" s="152"/>
       <c r="D176" s="158"/>
       <c r="E176" s="152"/>
       <c r="F176" s="84" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -4063,14 +4077,14 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" s="149" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B179" s="156"/>
       <c r="C179" s="153"/>
       <c r="D179" s="159"/>
       <c r="E179" s="153"/>
-      <c r="F179" s="161" t="s">
-        <v>216</v>
+      <c r="F179" s="84" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -4079,23 +4093,27 @@
       <c r="C180" s="153"/>
       <c r="D180" s="159"/>
       <c r="E180" s="153"/>
-      <c r="F180" s="162"/>
-    </row>
-    <row r="181" spans="1:6">
+      <c r="F180" s="85"/>
+    </row>
+    <row r="181" spans="1:6" ht="15.75" thickBot="1">
       <c r="A181" s="149"/>
       <c r="B181" s="156"/>
       <c r="C181" s="153"/>
       <c r="D181" s="159"/>
       <c r="E181" s="153"/>
-      <c r="F181" s="162"/>
+      <c r="F181" s="86"/>
     </row>
     <row r="182" spans="1:6">
-      <c r="A182" s="149"/>
-      <c r="B182" s="156"/>
-      <c r="C182" s="153"/>
-      <c r="D182" s="159"/>
-      <c r="E182" s="153"/>
-      <c r="F182" s="162"/>
+      <c r="A182" s="151" t="s">
+        <v>208</v>
+      </c>
+      <c r="B182" s="155"/>
+      <c r="C182" s="152"/>
+      <c r="D182" s="158"/>
+      <c r="E182" s="152"/>
+      <c r="F182" s="84" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="149"/>
@@ -4103,52 +4121,108 @@
       <c r="C183" s="153"/>
       <c r="D183" s="159"/>
       <c r="E183" s="153"/>
-      <c r="F183" s="162"/>
-    </row>
-    <row r="184" spans="1:6">
-      <c r="A184" s="149"/>
-      <c r="B184" s="156"/>
-      <c r="C184" s="153"/>
-      <c r="D184" s="159"/>
-      <c r="E184" s="153"/>
-      <c r="F184" s="162"/>
+      <c r="F183" s="85"/>
+    </row>
+    <row r="184" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A184" s="150"/>
+      <c r="B184" s="157"/>
+      <c r="C184" s="154"/>
+      <c r="D184" s="160"/>
+      <c r="E184" s="154"/>
+      <c r="F184" s="86"/>
     </row>
     <row r="185" spans="1:6">
-      <c r="A185" s="149"/>
+      <c r="A185" s="149" t="s">
+        <v>209</v>
+      </c>
       <c r="B185" s="156"/>
       <c r="C185" s="153"/>
       <c r="D185" s="159"/>
       <c r="E185" s="153"/>
-      <c r="F185" s="162"/>
-    </row>
-    <row r="186" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A186" s="150"/>
-      <c r="B186" s="157"/>
-      <c r="C186" s="154"/>
-      <c r="D186" s="160"/>
-      <c r="E186" s="154"/>
-      <c r="F186" s="163"/>
+      <c r="F185" s="161" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="149"/>
+      <c r="B186" s="156"/>
+      <c r="C186" s="153"/>
+      <c r="D186" s="159"/>
+      <c r="E186" s="153"/>
+      <c r="F186" s="162"/>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="149"/>
+      <c r="B187" s="156"/>
+      <c r="C187" s="153"/>
+      <c r="D187" s="159"/>
+      <c r="E187" s="153"/>
+      <c r="F187" s="162"/>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="149"/>
+      <c r="B188" s="156"/>
+      <c r="C188" s="153"/>
+      <c r="D188" s="159"/>
+      <c r="E188" s="153"/>
+      <c r="F188" s="162"/>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="149"/>
+      <c r="B189" s="156"/>
+      <c r="C189" s="153"/>
+      <c r="D189" s="159"/>
+      <c r="E189" s="153"/>
+      <c r="F189" s="162"/>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="149"/>
+      <c r="B190" s="156"/>
+      <c r="C190" s="153"/>
+      <c r="D190" s="159"/>
+      <c r="E190" s="153"/>
+      <c r="F190" s="162"/>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="149"/>
+      <c r="B191" s="156"/>
+      <c r="C191" s="153"/>
+      <c r="D191" s="159"/>
+      <c r="E191" s="153"/>
+      <c r="F191" s="162"/>
+    </row>
+    <row r="192" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A192" s="150"/>
+      <c r="B192" s="157"/>
+      <c r="C192" s="154"/>
+      <c r="D192" s="160"/>
+      <c r="E192" s="154"/>
+      <c r="F192" s="163"/>
     </row>
   </sheetData>
-  <mergeCells count="88">
-    <mergeCell ref="A179:A186"/>
+  <mergeCells count="92">
+    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="F164:F166"/>
+    <mergeCell ref="A161:A163"/>
     <mergeCell ref="F161:F163"/>
-    <mergeCell ref="F164:F166"/>
+    <mergeCell ref="A185:A192"/>
     <mergeCell ref="F167:F169"/>
     <mergeCell ref="F170:F172"/>
     <mergeCell ref="F173:F175"/>
     <mergeCell ref="F176:F178"/>
-    <mergeCell ref="F179:F186"/>
-    <mergeCell ref="A164:A166"/>
-    <mergeCell ref="A167:A169"/>
+    <mergeCell ref="F179:F181"/>
+    <mergeCell ref="F182:F184"/>
+    <mergeCell ref="F185:F192"/>
     <mergeCell ref="A170:A172"/>
     <mergeCell ref="A173:A175"/>
     <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="A182:A184"/>
     <mergeCell ref="F124:F130"/>
     <mergeCell ref="A117:A123"/>
     <mergeCell ref="E117:E123"/>
     <mergeCell ref="F117:F123"/>
-    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="A167:A169"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A155:A157"/>
     <mergeCell ref="F155:F157"/>

</xml_diff>

<commit_message>
auto alligned Z axis for cross_line
</commit_message>
<xml_diff>
--- a/description.xlsx
+++ b/description.xlsx
@@ -692,7 +692,8 @@
   <si>
     <t>вычисляет фрейм X ось которого совпадает с прямой  пересения XY плоскости Plate1 и  XY плоскости Plate2. 
 Плоскость XY нового фрейма совпадает с плоскостью XY Plate1. 
-Начало отсчета новой системы находится на проекции начала Plate1 на прямую пересечения плоскостей</t>
+Начало отсчета новой системы находится на проекции начала Plate1 на прямую пересечения плоскостей. Направление Z совпадает с направлением Z plate1
+ось X в направлении увеличения X исходной системы ( той относительно которой заданы все координаты)</t>
   </si>
 </sst>
 </file>
@@ -1913,8 +1914,8 @@
   <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D166" sqref="D166"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D145" sqref="D145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add description and listing
</commit_message>
<xml_diff>
--- a/description.xlsx
+++ b/description.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="225">
   <si>
     <t>SET_ORI(W,P,R)</t>
   </si>
@@ -674,12 +674,6 @@
     <t>MATH_LIB. Cross_Line (Plate1, Plate2: XYZWPR): XYZWPR</t>
   </si>
   <si>
-    <t>вычисляет фрейм X ось которого совпадает с прямой  пересения XY плоскости Plate1 и  XY плоскости Plate2. 
-Плоскость XY нового фрейма совпадает с плоскостью XY Plate1. 
-Начало отсчета новой системы находится на проекции начала Plate1 на прямую пересечения плоскостей. Направление Z совпадает с направлением Z plate1
-ось X в направлении увеличения X исходной системы ( той относительно которой заданы все координаты)</t>
-  </si>
-  <si>
     <t>S_elps(Z, D, a1, a2, end, turn)</t>
   </si>
   <si>
@@ -689,8 +683,11 @@
     <t>SET_IN_ST(till, rot).MR</t>
   </si>
   <si>
+    <t>MATH_LIB. Cross_PNT (Line_frame, Plane_frame: XYZWPR): XYZWPR</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">центр каждого сечения определяется как центр масс из центров 4 окружностей, ось Z направлена от 1 го сечения ко 2му,
+      <t xml:space="preserve">вычисляет точку пересения Z оcи LINE_frame c XY плоскостью Plate_frame
 </t>
     </r>
     <r>
@@ -702,12 +699,16 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">оси выровнены по PR[10] </t>
+      <t>НЕОБХОДИМО ЗАПРОГРАММИРОВАТЬ ПРОВЕРКУ КОРРЕКТНОГО РЕШЕНИЯ МАТРИЦЫ, НА СЛУЧАЙ ГЛАВНОГО ОПРЕДЕЛИТЕЛЯ 0 или если одна из поскостей проходит через начало координат</t>
     </r>
   </si>
   <si>
     <r>
-      <t>центр каждого сечения определяется как центр масс из центров 4 окружностей, плоскость XY определяется по 3м точка то</t>
+      <t xml:space="preserve">вычисляет фрейм X ось которого совпадает с прямой  пересения XY плоскости Plate1 и  XY плоскости Plate2. 
+Плоскость XY нового фрейма совпадает с плоскостью XY Plate1. 
+Начало отсчета новой системы находится на проекции начала Plate1 на прямую пересечения плоскостей. Направление Z совпадает с направлением Z plate1
+ось X в направлении увеличения X исходной системы ( той относительно которой заданы все координаты)
+ </t>
     </r>
     <r>
       <rPr>
@@ -718,22 +719,40 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>рца, оси паралельны Pr[10]</t>
+      <t>НЕОБХОДИМО ЗАПРОГРАММИРОВАТЬ ПРОВЕРКУ КОРРЕКТНОГО РЕШЕНИЯ МАТРИЦЫ, НА СЛУЧАЙ ГЛАВНОГО ОПРЕДЕЛИТЕЛЯ 0 или если одна из поскостей проходит через начало координат - скорее всего одно и тоже</t>
     </r>
   </si>
   <si>
-    <t>вычисляет точку пересения Z оcи LINE_frame c XY плоскостью Plate_frame
-НЕОБХОДИМО ЗАПРОГРАММИРОВАТЬ ПРОВЕРКУ КОРРЕКТНОГО РЕШЕНИЯ МАТРИЦЫ, НА СЛУЧАЙ ГЛАВНОГО ОПРЕДЕЛИТЕЛЯ 0 или если одна из поскостей проходит через начало координат</t>
-  </si>
-  <si>
-    <t>MATH_LIB. Cross_PNT (Line_frame, Plane_frame: XYZWPR): XYZWPR</t>
+    <t>Pr[10] - опорный фрейм - относительно строится ряд измерений</t>
+  </si>
+  <si>
+    <t>Pr[11] - фрейм оси заготовки</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">центр каждого сечения определяется как центр масс из центров 4 окружностей, ось Z проходит через центры сечений и ложительное направление совпадает с положительным направлением оси Z PR[10],
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ось X  параллельна  плоскости XZ  PR[10] </t>
+    </r>
+  </si>
+  <si>
+    <t>Плоскость XY совпадает с плоскостью торца, центр системы координат определяется как центр масс центров 4 окружностей построенных на проекциях измерений на плоскость торца. Оси X и  Y параллельны и сонаправлены с плоскостями XZ и YZ pr[10] соответсвенно</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -770,6 +789,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1213,7 +1239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1485,15 +1511,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1650,6 +1667,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1952,8 +1970,8 @@
   <dimension ref="A1:I199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F168" sqref="F168:F170"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F96" sqref="F96:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2036,7 +2054,7 @@
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1">
       <c r="A7" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -2130,7 +2148,7 @@
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1">
       <c r="A14" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -3121,8 +3139,8 @@
       <c r="E89" s="19"/>
       <c r="F89" s="110"/>
     </row>
-    <row r="90" spans="1:6" ht="45" customHeight="1">
-      <c r="A90" s="111" t="s">
+    <row r="90" spans="1:6" ht="45.75" customHeight="1">
+      <c r="A90" s="91" t="s">
         <v>168</v>
       </c>
       <c r="B90" s="15" t="s">
@@ -3134,11 +3152,11 @@
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="58" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A91" s="112"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A91" s="92"/>
       <c r="B91" s="9" t="s">
         <v>173</v>
       </c>
@@ -3149,8 +3167,8 @@
       <c r="E91" s="1"/>
       <c r="F91" s="59"/>
     </row>
-    <row r="92" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A92" s="113"/>
+    <row r="92" spans="1:6" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A92" s="93"/>
       <c r="B92" s="25"/>
       <c r="C92" s="17" t="s">
         <v>47</v>
@@ -3159,8 +3177,8 @@
       <c r="E92" s="4"/>
       <c r="F92" s="60"/>
     </row>
-    <row r="93" spans="1:6" ht="30" customHeight="1">
-      <c r="A93" s="111" t="s">
+    <row r="93" spans="1:6" ht="58.5" customHeight="1">
+      <c r="A93" s="91" t="s">
         <v>178</v>
       </c>
       <c r="B93" s="15" t="s">
@@ -3172,11 +3190,11 @@
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="58" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="30" customHeight="1">
-      <c r="A94" s="112"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="58.5" customHeight="1">
+      <c r="A94" s="92"/>
       <c r="B94" s="9" t="s">
         <v>179</v>
       </c>
@@ -3185,8 +3203,8 @@
       <c r="E94" s="1"/>
       <c r="F94" s="59"/>
     </row>
-    <row r="95" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A95" s="113"/>
+    <row r="95" spans="1:6" ht="58.5" customHeight="1" thickBot="1">
+      <c r="A95" s="93"/>
       <c r="B95" s="25"/>
       <c r="C95" s="17" t="s">
         <v>47</v>
@@ -3250,17 +3268,17 @@
       <c r="F100" s="60"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A101" s="116" t="s">
+      <c r="A101" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="B101" s="116"/>
-      <c r="C101" s="116"/>
-      <c r="D101" s="116"/>
-      <c r="E101" s="116"/>
-      <c r="F101" s="116"/>
+      <c r="B101" s="113"/>
+      <c r="C101" s="113"/>
+      <c r="D101" s="113"/>
+      <c r="E101" s="113"/>
+      <c r="F101" s="113"/>
     </row>
     <row r="102" spans="1:6" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A102" s="114" t="s">
+      <c r="A102" s="111" t="s">
         <v>50</v>
       </c>
       <c r="B102" s="3"/>
@@ -3276,7 +3294,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A103" s="115"/>
+      <c r="A103" s="112"/>
       <c r="B103" s="1"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8" t="s">
@@ -3285,10 +3303,10 @@
       <c r="E103" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F103" s="118"/>
+      <c r="F103" s="115"/>
     </row>
     <row r="104" spans="1:6" ht="30" customHeight="1">
-      <c r="A104" s="115"/>
+      <c r="A104" s="112"/>
       <c r="B104" s="1"/>
       <c r="C104" s="8"/>
       <c r="D104" s="9" t="s">
@@ -3297,10 +3315,10 @@
       <c r="E104" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F104" s="118"/>
+      <c r="F104" s="115"/>
     </row>
     <row r="105" spans="1:6" ht="30" customHeight="1">
-      <c r="A105" s="115"/>
+      <c r="A105" s="112"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="8" t="s">
@@ -3309,10 +3327,10 @@
       <c r="E105" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F105" s="118"/>
+      <c r="F105" s="115"/>
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1">
-      <c r="A106" s="115"/>
+      <c r="A106" s="112"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="8" t="s">
@@ -3321,10 +3339,10 @@
       <c r="E106" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F106" s="118"/>
+      <c r="F106" s="115"/>
     </row>
     <row r="107" spans="1:6" ht="15" customHeight="1">
-      <c r="A107" s="115"/>
+      <c r="A107" s="112"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="8" t="s">
@@ -3333,10 +3351,10 @@
       <c r="E107" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F107" s="118"/>
+      <c r="F107" s="115"/>
     </row>
     <row r="108" spans="1:6" ht="15" customHeight="1">
-      <c r="A108" s="115"/>
+      <c r="A108" s="112"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="8" t="s">
@@ -3345,10 +3363,10 @@
       <c r="E108" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F108" s="118"/>
+      <c r="F108" s="115"/>
     </row>
     <row r="109" spans="1:6" ht="15" customHeight="1">
-      <c r="A109" s="115"/>
+      <c r="A109" s="112"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="9" t="s">
@@ -3357,10 +3375,10 @@
       <c r="E109" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F109" s="118"/>
+      <c r="F109" s="115"/>
     </row>
     <row r="110" spans="1:6" ht="15" customHeight="1">
-      <c r="A110" s="115"/>
+      <c r="A110" s="112"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="9" t="s">
@@ -3369,10 +3387,10 @@
       <c r="E110" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F110" s="118"/>
+      <c r="F110" s="115"/>
     </row>
     <row r="111" spans="1:6" ht="15" customHeight="1">
-      <c r="A111" s="115"/>
+      <c r="A111" s="112"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="9" t="s">
@@ -3381,50 +3399,50 @@
       <c r="E111" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F111" s="118"/>
+      <c r="F111" s="115"/>
     </row>
     <row r="112" spans="1:6" ht="15" customHeight="1">
-      <c r="A112" s="115"/>
+      <c r="A112" s="112"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="18" t="s">
         <v>187</v>
       </c>
       <c r="E112" s="19"/>
-      <c r="F112" s="118"/>
+      <c r="F112" s="115"/>
     </row>
     <row r="113" spans="1:6" ht="15" customHeight="1">
-      <c r="A113" s="115"/>
+      <c r="A113" s="112"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="18" t="s">
         <v>186</v>
       </c>
       <c r="E113" s="19"/>
-      <c r="F113" s="118"/>
+      <c r="F113" s="115"/>
     </row>
     <row r="114" spans="1:6" ht="15" customHeight="1">
-      <c r="A114" s="115"/>
+      <c r="A114" s="112"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="18" t="s">
         <v>185</v>
       </c>
       <c r="E114" s="19"/>
-      <c r="F114" s="118"/>
+      <c r="F114" s="115"/>
     </row>
     <row r="115" spans="1:6">
-      <c r="A115" s="115"/>
+      <c r="A115" s="112"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="18" t="s">
         <v>184</v>
       </c>
       <c r="E115" s="19"/>
-      <c r="F115" s="118"/>
+      <c r="F115" s="115"/>
     </row>
     <row r="116" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A116" s="117"/>
+      <c r="A116" s="114"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="18"/>
@@ -3432,8 +3450,8 @@
       <c r="F116" s="110"/>
     </row>
     <row r="117" spans="1:6" ht="30" customHeight="1">
-      <c r="A117" s="119" t="s">
-        <v>216</v>
+      <c r="A117" s="116" t="s">
+        <v>215</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>19</v>
@@ -3452,7 +3470,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" ht="30" customHeight="1">
-      <c r="A118" s="120"/>
+      <c r="A118" s="117"/>
       <c r="B118" s="1" t="s">
         <v>22</v>
       </c>
@@ -3466,7 +3484,7 @@
       <c r="F118" s="53"/>
     </row>
     <row r="119" spans="1:6" ht="30" customHeight="1">
-      <c r="A119" s="120"/>
+      <c r="A119" s="117"/>
       <c r="B119" s="1" t="s">
         <v>20</v>
       </c>
@@ -3480,7 +3498,7 @@
       <c r="F119" s="53"/>
     </row>
     <row r="120" spans="1:6" ht="30" customHeight="1">
-      <c r="A120" s="120"/>
+      <c r="A120" s="117"/>
       <c r="B120" s="1" t="s">
         <v>21</v>
       </c>
@@ -3492,7 +3510,7 @@
       <c r="F120" s="53"/>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1">
-      <c r="A121" s="120"/>
+      <c r="A121" s="117"/>
       <c r="B121" s="1" t="s">
         <v>23</v>
       </c>
@@ -3504,7 +3522,7 @@
       <c r="F121" s="53"/>
     </row>
     <row r="122" spans="1:6" ht="15" customHeight="1">
-      <c r="A122" s="120"/>
+      <c r="A122" s="117"/>
       <c r="B122" s="1" t="s">
         <v>24</v>
       </c>
@@ -3516,7 +3534,7 @@
       <c r="F122" s="53"/>
     </row>
     <row r="123" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A123" s="120"/>
+      <c r="A123" s="117"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="29" t="s">
@@ -3526,7 +3544,7 @@
       <c r="F123" s="54"/>
     </row>
     <row r="124" spans="1:6" ht="30" customHeight="1">
-      <c r="A124" s="114" t="s">
+      <c r="A124" s="111" t="s">
         <v>191</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -3546,7 +3564,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" ht="30" customHeight="1">
-      <c r="A125" s="115"/>
+      <c r="A125" s="112"/>
       <c r="B125" s="1" t="s">
         <v>22</v>
       </c>
@@ -3560,7 +3578,7 @@
       <c r="F125" s="53"/>
     </row>
     <row r="126" spans="1:6" ht="30" customHeight="1">
-      <c r="A126" s="115"/>
+      <c r="A126" s="112"/>
       <c r="B126" s="1" t="s">
         <v>20</v>
       </c>
@@ -3574,7 +3592,7 @@
       <c r="F126" s="53"/>
     </row>
     <row r="127" spans="1:6" ht="30" customHeight="1">
-      <c r="A127" s="115"/>
+      <c r="A127" s="112"/>
       <c r="B127" s="1" t="s">
         <v>21</v>
       </c>
@@ -3586,7 +3604,7 @@
       <c r="F127" s="53"/>
     </row>
     <row r="128" spans="1:6" ht="15" customHeight="1">
-      <c r="A128" s="115"/>
+      <c r="A128" s="112"/>
       <c r="B128" s="1" t="s">
         <v>23</v>
       </c>
@@ -3598,7 +3616,7 @@
       <c r="F128" s="53"/>
     </row>
     <row r="129" spans="1:9" ht="15" customHeight="1">
-      <c r="A129" s="115"/>
+      <c r="A129" s="112"/>
       <c r="B129" s="1" t="s">
         <v>24</v>
       </c>
@@ -3610,7 +3628,7 @@
       <c r="F129" s="53"/>
     </row>
     <row r="130" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A130" s="115"/>
+      <c r="A130" s="112"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="29" t="s">
@@ -3620,7 +3638,7 @@
       <c r="F130" s="54"/>
     </row>
     <row r="131" spans="1:9" ht="30" customHeight="1">
-      <c r="A131" s="114" t="s">
+      <c r="A131" s="111" t="s">
         <v>192</v>
       </c>
       <c r="B131" s="3" t="s">
@@ -3640,7 +3658,7 @@
       </c>
     </row>
     <row r="132" spans="1:9" ht="30" customHeight="1">
-      <c r="A132" s="115"/>
+      <c r="A132" s="112"/>
       <c r="B132" s="1" t="s">
         <v>22</v>
       </c>
@@ -3654,7 +3672,7 @@
       <c r="F132" s="53"/>
     </row>
     <row r="133" spans="1:9" ht="30" customHeight="1">
-      <c r="A133" s="115"/>
+      <c r="A133" s="112"/>
       <c r="B133" s="1" t="s">
         <v>20</v>
       </c>
@@ -3668,7 +3686,7 @@
       <c r="F133" s="53"/>
     </row>
     <row r="134" spans="1:9" ht="30" customHeight="1">
-      <c r="A134" s="115"/>
+      <c r="A134" s="112"/>
       <c r="B134" s="1" t="s">
         <v>21</v>
       </c>
@@ -3680,7 +3698,7 @@
       <c r="F134" s="53"/>
     </row>
     <row r="135" spans="1:9" ht="15" customHeight="1">
-      <c r="A135" s="115"/>
+      <c r="A135" s="112"/>
       <c r="B135" s="1" t="s">
         <v>23</v>
       </c>
@@ -3692,7 +3710,7 @@
       <c r="F135" s="53"/>
     </row>
     <row r="136" spans="1:9" ht="15" customHeight="1">
-      <c r="A136" s="115"/>
+      <c r="A136" s="112"/>
       <c r="B136" s="1" t="s">
         <v>24</v>
       </c>
@@ -3704,7 +3722,7 @@
       <c r="F136" s="53"/>
     </row>
     <row r="137" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A137" s="115"/>
+      <c r="A137" s="112"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="29" t="s">
@@ -3855,7 +3873,7 @@
       <c r="F149" s="54"/>
     </row>
     <row r="150" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A150" s="124" t="s">
+      <c r="A150" s="121" t="s">
         <v>51</v>
       </c>
       <c r="B150" s="23" t="s">
@@ -3869,7 +3887,7 @@
       </c>
     </row>
     <row r="151" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A151" s="125"/>
+      <c r="A151" s="122"/>
       <c r="B151" s="16"/>
       <c r="C151" s="17"/>
       <c r="D151" s="17"/>
@@ -4040,14 +4058,14 @@
     </row>
     <row r="168" spans="1:6" ht="63.75" customHeight="1">
       <c r="A168" s="103" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B168" s="15"/>
       <c r="C168" s="14"/>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
       <c r="F168" s="72" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="63.75" customHeight="1">
@@ -4066,7 +4084,7 @@
       <c r="E170" s="17"/>
       <c r="F170" s="74"/>
     </row>
-    <row r="171" spans="1:6" ht="60" customHeight="1">
+    <row r="171" spans="1:6" ht="94.5" customHeight="1">
       <c r="A171" s="103" t="s">
         <v>214</v>
       </c>
@@ -4074,28 +4092,28 @@
       <c r="C171" s="14"/>
       <c r="D171" s="14"/>
       <c r="E171" s="14"/>
-      <c r="F171" s="126" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="60" customHeight="1">
+      <c r="F171" s="123" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="94.5" customHeight="1">
       <c r="A172" s="104"/>
       <c r="B172" s="21"/>
       <c r="C172" s="31"/>
       <c r="D172" s="31"/>
       <c r="E172" s="31"/>
-      <c r="F172" s="127"/>
-    </row>
-    <row r="173" spans="1:6" ht="60" customHeight="1" thickBot="1">
+      <c r="F172" s="124"/>
+    </row>
+    <row r="173" spans="1:6" ht="94.5" customHeight="1" thickBot="1">
       <c r="A173" s="105"/>
       <c r="B173" s="16"/>
       <c r="C173" s="17"/>
       <c r="D173" s="17"/>
       <c r="E173" s="17"/>
-      <c r="F173" s="128"/>
+      <c r="F173" s="125"/>
     </row>
     <row r="174" spans="1:6" ht="15" customHeight="1">
-      <c r="A174" s="121" t="s">
+      <c r="A174" s="118" t="s">
         <v>200</v>
       </c>
       <c r="B174" s="40"/>
@@ -4107,7 +4125,7 @@
       </c>
     </row>
     <row r="175" spans="1:6">
-      <c r="A175" s="122"/>
+      <c r="A175" s="119"/>
       <c r="B175" s="41"/>
       <c r="C175" s="38"/>
       <c r="D175" s="44"/>
@@ -4115,7 +4133,7 @@
       <c r="F175" s="73"/>
     </row>
     <row r="176" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A176" s="123"/>
+      <c r="A176" s="120"/>
       <c r="B176" s="42"/>
       <c r="C176" s="39"/>
       <c r="D176" s="45"/>
@@ -4123,7 +4141,7 @@
       <c r="F176" s="74"/>
     </row>
     <row r="177" spans="1:6">
-      <c r="A177" s="121" t="s">
+      <c r="A177" s="118" t="s">
         <v>201</v>
       </c>
       <c r="B177" s="40"/>
@@ -4135,7 +4153,7 @@
       </c>
     </row>
     <row r="178" spans="1:6">
-      <c r="A178" s="122"/>
+      <c r="A178" s="119"/>
       <c r="B178" s="41"/>
       <c r="C178" s="38"/>
       <c r="D178" s="44"/>
@@ -4143,7 +4161,7 @@
       <c r="F178" s="73"/>
     </row>
     <row r="179" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A179" s="123"/>
+      <c r="A179" s="120"/>
       <c r="B179" s="42"/>
       <c r="C179" s="39"/>
       <c r="D179" s="45"/>
@@ -4151,7 +4169,7 @@
       <c r="F179" s="74"/>
     </row>
     <row r="180" spans="1:6">
-      <c r="A180" s="122" t="s">
+      <c r="A180" s="119" t="s">
         <v>202</v>
       </c>
       <c r="B180" s="41"/>
@@ -4163,7 +4181,7 @@
       </c>
     </row>
     <row r="181" spans="1:6">
-      <c r="A181" s="122"/>
+      <c r="A181" s="119"/>
       <c r="B181" s="41"/>
       <c r="C181" s="38"/>
       <c r="D181" s="44"/>
@@ -4171,7 +4189,7 @@
       <c r="F181" s="73"/>
     </row>
     <row r="182" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A182" s="122"/>
+      <c r="A182" s="119"/>
       <c r="B182" s="41"/>
       <c r="C182" s="38"/>
       <c r="D182" s="44"/>
@@ -4179,7 +4197,7 @@
       <c r="F182" s="74"/>
     </row>
     <row r="183" spans="1:6">
-      <c r="A183" s="121" t="s">
+      <c r="A183" s="118" t="s">
         <v>203</v>
       </c>
       <c r="B183" s="40"/>
@@ -4191,7 +4209,7 @@
       </c>
     </row>
     <row r="184" spans="1:6">
-      <c r="A184" s="122"/>
+      <c r="A184" s="119"/>
       <c r="B184" s="41"/>
       <c r="C184" s="38"/>
       <c r="D184" s="44"/>
@@ -4199,7 +4217,7 @@
       <c r="F184" s="73"/>
     </row>
     <row r="185" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A185" s="123"/>
+      <c r="A185" s="120"/>
       <c r="B185" s="42"/>
       <c r="C185" s="39"/>
       <c r="D185" s="45"/>
@@ -4207,7 +4225,7 @@
       <c r="F185" s="74"/>
     </row>
     <row r="186" spans="1:6">
-      <c r="A186" s="122" t="s">
+      <c r="A186" s="119" t="s">
         <v>204</v>
       </c>
       <c r="B186" s="41"/>
@@ -4219,7 +4237,7 @@
       </c>
     </row>
     <row r="187" spans="1:6">
-      <c r="A187" s="122"/>
+      <c r="A187" s="119"/>
       <c r="B187" s="41"/>
       <c r="C187" s="38"/>
       <c r="D187" s="44"/>
@@ -4227,7 +4245,7 @@
       <c r="F187" s="73"/>
     </row>
     <row r="188" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A188" s="122"/>
+      <c r="A188" s="119"/>
       <c r="B188" s="41"/>
       <c r="C188" s="38"/>
       <c r="D188" s="44"/>
@@ -4235,7 +4253,7 @@
       <c r="F188" s="74"/>
     </row>
     <row r="189" spans="1:6">
-      <c r="A189" s="121" t="s">
+      <c r="A189" s="118" t="s">
         <v>205</v>
       </c>
       <c r="B189" s="40"/>
@@ -4247,7 +4265,7 @@
       </c>
     </row>
     <row r="190" spans="1:6">
-      <c r="A190" s="122"/>
+      <c r="A190" s="119"/>
       <c r="B190" s="41"/>
       <c r="C190" s="38"/>
       <c r="D190" s="44"/>
@@ -4255,7 +4273,7 @@
       <c r="F190" s="73"/>
     </row>
     <row r="191" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A191" s="123"/>
+      <c r="A191" s="120"/>
       <c r="B191" s="42"/>
       <c r="C191" s="39"/>
       <c r="D191" s="45"/>
@@ -4263,72 +4281,72 @@
       <c r="F191" s="74"/>
     </row>
     <row r="192" spans="1:6">
-      <c r="A192" s="122" t="s">
+      <c r="A192" s="119" t="s">
         <v>206</v>
       </c>
       <c r="B192" s="41"/>
       <c r="C192" s="38"/>
       <c r="D192" s="44"/>
       <c r="E192" s="38"/>
-      <c r="F192" s="126" t="s">
+      <c r="F192" s="123" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="193" spans="1:6">
-      <c r="A193" s="122"/>
+      <c r="A193" s="119"/>
       <c r="B193" s="41"/>
       <c r="C193" s="38"/>
       <c r="D193" s="44"/>
       <c r="E193" s="38"/>
-      <c r="F193" s="127"/>
+      <c r="F193" s="124"/>
     </row>
     <row r="194" spans="1:6">
-      <c r="A194" s="122"/>
+      <c r="A194" s="119"/>
       <c r="B194" s="41"/>
       <c r="C194" s="38"/>
       <c r="D194" s="44"/>
       <c r="E194" s="38"/>
-      <c r="F194" s="127"/>
+      <c r="F194" s="124"/>
     </row>
     <row r="195" spans="1:6">
-      <c r="A195" s="122"/>
+      <c r="A195" s="119"/>
       <c r="B195" s="41"/>
       <c r="C195" s="38"/>
       <c r="D195" s="44"/>
       <c r="E195" s="38"/>
-      <c r="F195" s="127"/>
+      <c r="F195" s="124"/>
     </row>
     <row r="196" spans="1:6">
-      <c r="A196" s="122"/>
+      <c r="A196" s="119"/>
       <c r="B196" s="41"/>
       <c r="C196" s="38"/>
       <c r="D196" s="44"/>
       <c r="E196" s="38"/>
-      <c r="F196" s="127"/>
+      <c r="F196" s="124"/>
     </row>
     <row r="197" spans="1:6">
-      <c r="A197" s="122"/>
+      <c r="A197" s="119"/>
       <c r="B197" s="41"/>
       <c r="C197" s="38"/>
       <c r="D197" s="44"/>
       <c r="E197" s="38"/>
-      <c r="F197" s="127"/>
+      <c r="F197" s="124"/>
     </row>
     <row r="198" spans="1:6">
-      <c r="A198" s="122"/>
+      <c r="A198" s="119"/>
       <c r="B198" s="41"/>
       <c r="C198" s="38"/>
       <c r="D198" s="44"/>
       <c r="E198" s="38"/>
-      <c r="F198" s="127"/>
+      <c r="F198" s="124"/>
     </row>
     <row r="199" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A199" s="123"/>
+      <c r="A199" s="120"/>
       <c r="B199" s="42"/>
       <c r="C199" s="39"/>
       <c r="D199" s="45"/>
       <c r="E199" s="39"/>
-      <c r="F199" s="128"/>
+      <c r="F199" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="95">
@@ -4486,7 +4504,7 @@
       <c r="F2" s="76"/>
     </row>
     <row r="3" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="129" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4506,7 +4524,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A4" s="133"/>
+      <c r="A4" s="130"/>
       <c r="B4" s="1" t="s">
         <v>95</v>
       </c>
@@ -4520,7 +4538,7 @@
       <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A5" s="134"/>
+      <c r="A5" s="131"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="9" t="s">
@@ -4532,7 +4550,7 @@
       <c r="F5" s="53"/>
     </row>
     <row r="6" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A6" s="134"/>
+      <c r="A6" s="131"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="8" t="s">
@@ -4544,7 +4562,7 @@
       <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A7" s="134"/>
+      <c r="A7" s="131"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="8" t="s">
@@ -4556,7 +4574,7 @@
       <c r="F7" s="53"/>
     </row>
     <row r="8" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A8" s="134"/>
+      <c r="A8" s="131"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="8" t="s">
@@ -4568,7 +4586,7 @@
       <c r="F8" s="53"/>
     </row>
     <row r="9" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A9" s="134"/>
+      <c r="A9" s="131"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="13" t="s">
@@ -4580,7 +4598,7 @@
       <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A10" s="132" t="s">
+      <c r="A10" s="129" t="s">
         <v>96</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -4600,7 +4618,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A11" s="133"/>
+      <c r="A11" s="130"/>
       <c r="B11" s="1" t="s">
         <v>95</v>
       </c>
@@ -4614,7 +4632,7 @@
       <c r="F11" s="53"/>
     </row>
     <row r="12" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A12" s="134"/>
+      <c r="A12" s="131"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="9" t="s">
@@ -4626,7 +4644,7 @@
       <c r="F12" s="53"/>
     </row>
     <row r="13" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A13" s="134"/>
+      <c r="A13" s="131"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="8" t="s">
@@ -4638,7 +4656,7 @@
       <c r="F13" s="53"/>
     </row>
     <row r="14" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A14" s="134"/>
+      <c r="A14" s="131"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="8" t="s">
@@ -4650,7 +4668,7 @@
       <c r="F14" s="53"/>
     </row>
     <row r="15" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A15" s="134"/>
+      <c r="A15" s="131"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="8" t="s">
@@ -4662,7 +4680,7 @@
       <c r="F15" s="53"/>
     </row>
     <row r="16" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A16" s="134"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="13" t="s">
@@ -4674,7 +4692,7 @@
       <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A17" s="132" t="s">
+      <c r="A17" s="129" t="s">
         <v>99</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -4694,7 +4712,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A18" s="133"/>
+      <c r="A18" s="130"/>
       <c r="B18" s="1" t="s">
         <v>95</v>
       </c>
@@ -4708,7 +4726,7 @@
       <c r="F18" s="53"/>
     </row>
     <row r="19" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A19" s="134"/>
+      <c r="A19" s="131"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="9" t="s">
@@ -4720,7 +4738,7 @@
       <c r="F19" s="53"/>
     </row>
     <row r="20" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A20" s="134"/>
+      <c r="A20" s="131"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="8" t="s">
@@ -4732,7 +4750,7 @@
       <c r="F20" s="53"/>
     </row>
     <row r="21" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A21" s="134"/>
+      <c r="A21" s="131"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="8" t="s">
@@ -4744,7 +4762,7 @@
       <c r="F21" s="53"/>
     </row>
     <row r="22" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A22" s="134"/>
+      <c r="A22" s="131"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="8" t="s">
@@ -4756,7 +4774,7 @@
       <c r="F22" s="53"/>
     </row>
     <row r="23" spans="1:8" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A23" s="134"/>
+      <c r="A23" s="131"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="13" t="s">
@@ -4768,7 +4786,7 @@
       <c r="F23" s="53"/>
     </row>
     <row r="24" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A24" s="132" t="s">
+      <c r="A24" s="129" t="s">
         <v>68</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -4788,7 +4806,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A25" s="133"/>
+      <c r="A25" s="130"/>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
@@ -4802,7 +4820,7 @@
       <c r="F25" s="53"/>
     </row>
     <row r="26" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A26" s="133"/>
+      <c r="A26" s="130"/>
       <c r="B26" s="1" t="s">
         <v>20</v>
       </c>
@@ -4816,7 +4834,7 @@
       <c r="F26" s="53"/>
     </row>
     <row r="27" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A27" s="133"/>
+      <c r="A27" s="130"/>
       <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
@@ -4828,7 +4846,7 @@
       <c r="F27" s="53"/>
     </row>
     <row r="28" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A28" s="133"/>
+      <c r="A28" s="130"/>
       <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
@@ -4840,7 +4858,7 @@
       <c r="F28" s="53"/>
     </row>
     <row r="29" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A29" s="133"/>
+      <c r="A29" s="130"/>
       <c r="B29" s="1" t="s">
         <v>24</v>
       </c>
@@ -4852,7 +4870,7 @@
       <c r="F29" s="53"/>
     </row>
     <row r="30" spans="1:8" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A30" s="135"/>
+      <c r="A30" s="132"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="29" t="s">
@@ -4862,7 +4880,7 @@
       <c r="F30" s="54"/>
     </row>
     <row r="31" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A31" s="132" t="s">
+      <c r="A31" s="129" t="s">
         <v>147</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -4888,7 +4906,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A32" s="133"/>
+      <c r="A32" s="130"/>
       <c r="B32" s="1" t="s">
         <v>22</v>
       </c>
@@ -4905,7 +4923,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A33" s="133"/>
+      <c r="A33" s="130"/>
       <c r="B33" s="1" t="s">
         <v>20</v>
       </c>
@@ -4925,7 +4943,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A34" s="133"/>
+      <c r="A34" s="130"/>
       <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
@@ -4943,7 +4961,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A35" s="133"/>
+      <c r="A35" s="130"/>
       <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
@@ -4961,7 +4979,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A36" s="133"/>
+      <c r="A36" s="130"/>
       <c r="B36" s="1" t="s">
         <v>24</v>
       </c>
@@ -4979,7 +4997,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A37" s="134"/>
+      <c r="A37" s="131"/>
       <c r="B37" s="2" t="s">
         <v>132</v>
       </c>
@@ -4998,7 +5016,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A38" s="134"/>
+      <c r="A38" s="131"/>
       <c r="B38" s="2" t="s">
         <v>131</v>
       </c>
@@ -5017,7 +5035,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A39" s="134"/>
+      <c r="A39" s="131"/>
       <c r="B39" s="2" t="s">
         <v>130</v>
       </c>
@@ -5036,7 +5054,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A40" s="135"/>
+      <c r="A40" s="132"/>
       <c r="B40" s="4" t="s">
         <v>129</v>
       </c>
@@ -5051,7 +5069,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A41" s="163" t="s">
+      <c r="A41" s="160" t="s">
         <v>69</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -5071,7 +5089,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A42" s="164"/>
+      <c r="A42" s="161"/>
       <c r="B42" s="1" t="s">
         <v>70</v>
       </c>
@@ -5083,7 +5101,7 @@
       <c r="F42" s="53"/>
     </row>
     <row r="43" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A43" s="164"/>
+      <c r="A43" s="161"/>
       <c r="B43" s="1" t="s">
         <v>49</v>
       </c>
@@ -5095,7 +5113,7 @@
       <c r="F43" s="53"/>
     </row>
     <row r="44" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A44" s="164"/>
+      <c r="A44" s="161"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="8" t="s">
@@ -5105,7 +5123,7 @@
       <c r="F44" s="53"/>
     </row>
     <row r="45" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A45" s="164"/>
+      <c r="A45" s="161"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="8" t="s">
@@ -5115,7 +5133,7 @@
       <c r="F45" s="53"/>
     </row>
     <row r="46" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A46" s="164"/>
+      <c r="A46" s="161"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="8" t="s">
@@ -5125,7 +5143,7 @@
       <c r="F46" s="53"/>
     </row>
     <row r="47" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A47" s="165"/>
+      <c r="A47" s="162"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="29" t="s">
@@ -5135,13 +5153,13 @@
       <c r="F47" s="54"/>
     </row>
     <row r="48" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A48" s="132" t="s">
+      <c r="A48" s="129" t="s">
         <v>150</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="161" t="s">
+      <c r="C48" s="158" t="s">
         <v>45</v>
       </c>
       <c r="D48" s="15" t="s">
@@ -5155,11 +5173,11 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A49" s="133"/>
+      <c r="A49" s="130"/>
       <c r="B49" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="162"/>
+      <c r="C49" s="159"/>
       <c r="D49" s="9" t="s">
         <v>15</v>
       </c>
@@ -5167,7 +5185,7 @@
       <c r="F49" s="73"/>
     </row>
     <row r="50" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A50" s="133"/>
+      <c r="A50" s="130"/>
       <c r="B50" s="5" t="s">
         <v>29</v>
       </c>
@@ -5181,7 +5199,7 @@
       <c r="F50" s="73"/>
     </row>
     <row r="51" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A51" s="133"/>
+      <c r="A51" s="130"/>
       <c r="B51" s="24" t="s">
         <v>30</v>
       </c>
@@ -5195,7 +5213,7 @@
       <c r="F51" s="73"/>
     </row>
     <row r="52" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A52" s="133"/>
+      <c r="A52" s="130"/>
       <c r="B52" s="24" t="s">
         <v>31</v>
       </c>
@@ -5209,7 +5227,7 @@
       <c r="F52" s="73"/>
     </row>
     <row r="53" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A53" s="133"/>
+      <c r="A53" s="130"/>
       <c r="B53" s="24" t="s">
         <v>32</v>
       </c>
@@ -5221,7 +5239,7 @@
       <c r="F53" s="73"/>
     </row>
     <row r="54" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A54" s="133"/>
+      <c r="A54" s="130"/>
       <c r="B54" s="24" t="s">
         <v>33</v>
       </c>
@@ -5233,7 +5251,7 @@
       <c r="F54" s="73"/>
     </row>
     <row r="55" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A55" s="135"/>
+      <c r="A55" s="132"/>
       <c r="B55" s="25"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
@@ -5251,7 +5269,7 @@
       <c r="F56" s="75"/>
     </row>
     <row r="57" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A57" s="129" t="s">
+      <c r="A57" s="126" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="12" t="s">
@@ -5265,7 +5283,7 @@
       <c r="F57" s="58"/>
     </row>
     <row r="58" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A58" s="130"/>
+      <c r="A58" s="127"/>
       <c r="B58" s="8" t="s">
         <v>15</v>
       </c>
@@ -5277,7 +5295,7 @@
       <c r="F58" s="59"/>
     </row>
     <row r="59" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A59" s="136"/>
+      <c r="A59" s="133"/>
       <c r="B59" s="9" t="s">
         <v>10</v>
       </c>
@@ -5289,7 +5307,7 @@
       <c r="F59" s="59"/>
     </row>
     <row r="60" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A60" s="136"/>
+      <c r="A60" s="133"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -5297,7 +5315,7 @@
       <c r="F60" s="59"/>
     </row>
     <row r="61" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A61" s="131"/>
+      <c r="A61" s="128"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -5305,7 +5323,7 @@
       <c r="F61" s="60"/>
     </row>
     <row r="62" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A62" s="129" t="s">
+      <c r="A62" s="126" t="s">
         <v>12</v>
       </c>
       <c r="B62" s="3"/>
@@ -5319,7 +5337,7 @@
       <c r="F62" s="58"/>
     </row>
     <row r="63" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A63" s="130"/>
+      <c r="A63" s="127"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -5327,7 +5345,7 @@
       <c r="F63" s="59"/>
     </row>
     <row r="64" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A64" s="131"/>
+      <c r="A64" s="128"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -5335,7 +5353,7 @@
       <c r="F64" s="60"/>
     </row>
     <row r="65" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A65" s="129" t="s">
+      <c r="A65" s="126" t="s">
         <v>0</v>
       </c>
       <c r="B65" s="8" t="s">
@@ -5349,7 +5367,7 @@
       <c r="F65" s="58"/>
     </row>
     <row r="66" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A66" s="130"/>
+      <c r="A66" s="127"/>
       <c r="B66" s="8" t="s">
         <v>8</v>
       </c>
@@ -5361,7 +5379,7 @@
       <c r="F66" s="59"/>
     </row>
     <row r="67" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A67" s="131"/>
+      <c r="A67" s="128"/>
       <c r="B67" s="13" t="s">
         <v>9</v>
       </c>
@@ -5373,7 +5391,7 @@
       <c r="F67" s="60"/>
     </row>
     <row r="68" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A68" s="129" t="s">
+      <c r="A68" s="126" t="s">
         <v>42</v>
       </c>
       <c r="B68" s="9" t="s">
@@ -5387,7 +5405,7 @@
       <c r="F68" s="58"/>
     </row>
     <row r="69" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A69" s="130"/>
+      <c r="A69" s="127"/>
       <c r="B69" s="9" t="s">
         <v>40</v>
       </c>
@@ -5399,7 +5417,7 @@
       <c r="F69" s="59"/>
     </row>
     <row r="70" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A70" s="131"/>
+      <c r="A70" s="128"/>
       <c r="B70" s="9" t="s">
         <v>41</v>
       </c>
@@ -5509,7 +5527,7 @@
       <c r="F77" s="60"/>
     </row>
     <row r="78" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A78" s="152" t="s">
+      <c r="A78" s="149" t="s">
         <v>66</v>
       </c>
       <c r="B78" s="26" t="s">
@@ -5537,7 +5555,7 @@
       <c r="F79" s="98"/>
     </row>
     <row r="80" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A80" s="131"/>
+      <c r="A80" s="128"/>
       <c r="B80" s="25"/>
       <c r="C80" s="5" t="s">
         <v>67</v>
@@ -5547,7 +5565,7 @@
       <c r="F80" s="99"/>
     </row>
     <row r="81" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A81" s="129" t="s">
+      <c r="A81" s="126" t="s">
         <v>112</v>
       </c>
       <c r="B81" s="27" t="s">
@@ -5567,7 +5585,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A82" s="136"/>
+      <c r="A82" s="133"/>
       <c r="B82" s="28"/>
       <c r="C82" s="2" t="s">
         <v>67</v>
@@ -5577,7 +5595,7 @@
       <c r="F82" s="60"/>
     </row>
     <row r="83" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A83" s="129" t="s">
+      <c r="A83" s="126" t="s">
         <v>65</v>
       </c>
       <c r="B83" s="27" t="s">
@@ -5592,17 +5610,17 @@
       <c r="E83" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F83" s="153"/>
+      <c r="F83" s="150"/>
     </row>
     <row r="84" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A84" s="136"/>
+      <c r="A84" s="133"/>
       <c r="B84" s="28"/>
       <c r="C84" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="19"/>
-      <c r="F84" s="154"/>
+      <c r="F84" s="151"/>
     </row>
     <row r="85" spans="1:6" ht="33.75" customHeight="1">
       <c r="A85" s="55" t="s">
@@ -5679,7 +5697,7 @@
       <c r="F90" s="60"/>
     </row>
     <row r="91" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A91" s="149" t="s">
+      <c r="A91" s="146" t="s">
         <v>71</v>
       </c>
       <c r="B91" s="3"/>
@@ -5693,7 +5711,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A92" s="150"/>
+      <c r="A92" s="147"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
         <v>73</v>
@@ -5703,7 +5721,7 @@
       <c r="F92" s="59"/>
     </row>
     <row r="93" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A93" s="150"/>
+      <c r="A93" s="147"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
         <v>72</v>
@@ -5713,7 +5731,7 @@
       <c r="F93" s="59"/>
     </row>
     <row r="94" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A94" s="150"/>
+      <c r="A94" s="147"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
         <v>74</v>
@@ -5723,7 +5741,7 @@
       <c r="F94" s="59"/>
     </row>
     <row r="95" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A95" s="151"/>
+      <c r="A95" s="148"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4" t="s">
         <v>75</v>
@@ -5733,17 +5751,17 @@
       <c r="F95" s="60"/>
     </row>
     <row r="96" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A96" s="116" t="s">
+      <c r="A96" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="B96" s="116"/>
-      <c r="C96" s="116"/>
-      <c r="D96" s="116"/>
-      <c r="E96" s="116"/>
-      <c r="F96" s="116"/>
+      <c r="B96" s="113"/>
+      <c r="C96" s="113"/>
+      <c r="D96" s="113"/>
+      <c r="E96" s="113"/>
+      <c r="F96" s="113"/>
     </row>
     <row r="97" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A97" s="157" t="s">
+      <c r="A97" s="154" t="s">
         <v>50</v>
       </c>
       <c r="B97" s="3"/>
@@ -5754,12 +5772,12 @@
       <c r="E97" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F97" s="153" t="s">
+      <c r="F97" s="150" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A98" s="158"/>
+      <c r="A98" s="155"/>
       <c r="B98" s="1"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8" t="s">
@@ -5768,10 +5786,10 @@
       <c r="E98" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F98" s="160"/>
+      <c r="F98" s="157"/>
     </row>
     <row r="99" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A99" s="158"/>
+      <c r="A99" s="155"/>
       <c r="B99" s="1"/>
       <c r="C99" s="8"/>
       <c r="D99" s="9" t="s">
@@ -5780,10 +5798,10 @@
       <c r="E99" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F99" s="160"/>
+      <c r="F99" s="157"/>
     </row>
     <row r="100" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A100" s="158"/>
+      <c r="A100" s="155"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="8" t="s">
@@ -5792,10 +5810,10 @@
       <c r="E100" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F100" s="160"/>
+      <c r="F100" s="157"/>
     </row>
     <row r="101" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A101" s="158"/>
+      <c r="A101" s="155"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="8" t="s">
@@ -5804,10 +5822,10 @@
       <c r="E101" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F101" s="160"/>
+      <c r="F101" s="157"/>
     </row>
     <row r="102" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A102" s="158"/>
+      <c r="A102" s="155"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="8" t="s">
@@ -5816,10 +5834,10 @@
       <c r="E102" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F102" s="160"/>
+      <c r="F102" s="157"/>
     </row>
     <row r="103" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A103" s="158"/>
+      <c r="A103" s="155"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="8" t="s">
@@ -5828,10 +5846,10 @@
       <c r="E103" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F103" s="160"/>
+      <c r="F103" s="157"/>
     </row>
     <row r="104" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A104" s="158"/>
+      <c r="A104" s="155"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="9" t="s">
@@ -5840,10 +5858,10 @@
       <c r="E104" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F104" s="160"/>
+      <c r="F104" s="157"/>
     </row>
     <row r="105" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A105" s="158"/>
+      <c r="A105" s="155"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="9" t="s">
@@ -5852,10 +5870,10 @@
       <c r="E105" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F105" s="160"/>
+      <c r="F105" s="157"/>
     </row>
     <row r="106" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A106" s="158"/>
+      <c r="A106" s="155"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="9" t="s">
@@ -5864,26 +5882,26 @@
       <c r="E106" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F106" s="160"/>
+      <c r="F106" s="157"/>
     </row>
     <row r="107" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A107" s="159"/>
+      <c r="A107" s="156"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="18"/>
       <c r="E107" s="19"/>
-      <c r="F107" s="154"/>
+      <c r="F107" s="151"/>
     </row>
     <row r="108" spans="1:6" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A108" s="159"/>
+      <c r="A108" s="156"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="18"/>
       <c r="E108" s="19"/>
-      <c r="F108" s="154"/>
+      <c r="F108" s="151"/>
     </row>
     <row r="109" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A109" s="140" t="s">
+      <c r="A109" s="137" t="s">
         <v>138</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -5893,13 +5911,13 @@
         <v>26</v>
       </c>
       <c r="D109" s="12"/>
-      <c r="E109" s="143"/>
-      <c r="F109" s="146" t="s">
+      <c r="E109" s="140"/>
+      <c r="F109" s="143" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A110" s="141"/>
+      <c r="A110" s="138"/>
       <c r="B110" s="1" t="s">
         <v>131</v>
       </c>
@@ -5907,11 +5925,11 @@
         <v>148</v>
       </c>
       <c r="D110" s="8"/>
-      <c r="E110" s="144"/>
-      <c r="F110" s="147"/>
+      <c r="E110" s="141"/>
+      <c r="F110" s="144"/>
     </row>
     <row r="111" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A111" s="141"/>
+      <c r="A111" s="138"/>
       <c r="B111" s="1" t="s">
         <v>130</v>
       </c>
@@ -5919,11 +5937,11 @@
         <v>139</v>
       </c>
       <c r="D111" s="9"/>
-      <c r="E111" s="144"/>
-      <c r="F111" s="147"/>
+      <c r="E111" s="141"/>
+      <c r="F111" s="144"/>
     </row>
     <row r="112" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A112" s="141"/>
+      <c r="A112" s="138"/>
       <c r="B112" s="1" t="s">
         <v>129</v>
       </c>
@@ -5931,11 +5949,11 @@
         <v>140</v>
       </c>
       <c r="D112" s="8"/>
-      <c r="E112" s="144"/>
-      <c r="F112" s="147"/>
+      <c r="E112" s="141"/>
+      <c r="F112" s="144"/>
     </row>
     <row r="113" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A113" s="141"/>
+      <c r="A113" s="138"/>
       <c r="B113" s="1" t="s">
         <v>22</v>
       </c>
@@ -5943,11 +5961,11 @@
         <v>141</v>
       </c>
       <c r="D113" s="8"/>
-      <c r="E113" s="144"/>
-      <c r="F113" s="147"/>
+      <c r="E113" s="141"/>
+      <c r="F113" s="144"/>
     </row>
     <row r="114" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A114" s="141"/>
+      <c r="A114" s="138"/>
       <c r="B114" s="1" t="s">
         <v>23</v>
       </c>
@@ -5955,63 +5973,63 @@
         <v>142</v>
       </c>
       <c r="D114" s="8"/>
-      <c r="E114" s="144"/>
-      <c r="F114" s="147"/>
+      <c r="E114" s="141"/>
+      <c r="F114" s="144"/>
     </row>
     <row r="115" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A115" s="141"/>
+      <c r="A115" s="138"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D115" s="8"/>
-      <c r="E115" s="144"/>
-      <c r="F115" s="147"/>
+      <c r="E115" s="141"/>
+      <c r="F115" s="144"/>
       <c r="I115" s="36"/>
     </row>
     <row r="116" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A116" s="141"/>
+      <c r="A116" s="138"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D116" s="8"/>
-      <c r="E116" s="144"/>
-      <c r="F116" s="147"/>
+      <c r="E116" s="141"/>
+      <c r="F116" s="144"/>
       <c r="I116" s="36"/>
     </row>
     <row r="117" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A117" s="141"/>
+      <c r="A117" s="138"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D117" s="8"/>
-      <c r="E117" s="144"/>
-      <c r="F117" s="147"/>
+      <c r="E117" s="141"/>
+      <c r="F117" s="144"/>
       <c r="I117" s="36"/>
     </row>
     <row r="118" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A118" s="141"/>
+      <c r="A118" s="138"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1" t="s">
         <v>149</v>
       </c>
       <c r="D118" s="8"/>
-      <c r="E118" s="144"/>
-      <c r="F118" s="147"/>
+      <c r="E118" s="141"/>
+      <c r="F118" s="144"/>
       <c r="I118" s="36"/>
     </row>
     <row r="119" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A119" s="142"/>
+      <c r="A119" s="139"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="29"/>
-      <c r="E119" s="145"/>
-      <c r="F119" s="148"/>
+      <c r="E119" s="142"/>
+      <c r="F119" s="145"/>
     </row>
     <row r="120" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A120" s="155" t="s">
+      <c r="A120" s="152" t="s">
         <v>51</v>
       </c>
       <c r="B120" s="23" t="s">
@@ -6025,7 +6043,7 @@
       </c>
     </row>
     <row r="121" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A121" s="156"/>
+      <c r="A121" s="153"/>
       <c r="B121" s="16"/>
       <c r="C121" s="17"/>
       <c r="D121" s="17"/>
@@ -6067,7 +6085,7 @@
       <c r="F124" s="73"/>
     </row>
     <row r="125" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A125" s="137" t="s">
+      <c r="A125" s="134" t="s">
         <v>81</v>
       </c>
       <c r="B125" s="15" t="s">
@@ -6081,7 +6099,7 @@
       </c>
     </row>
     <row r="126" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A126" s="138"/>
+      <c r="A126" s="135"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -6089,7 +6107,7 @@
       <c r="F126" s="59"/>
     </row>
     <row r="127" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A127" s="138"/>
+      <c r="A127" s="135"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -6097,7 +6115,7 @@
       <c r="F127" s="59"/>
     </row>
     <row r="128" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A128" s="139"/>
+      <c r="A128" s="136"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -6247,10 +6265,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6380,6 +6398,16 @@
         <v>59</v>
       </c>
     </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="163" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="163" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>